<commit_message>
Refactor agenda items and update fitness documentation; remove outdated exercise routines and add new beta tester invitation details.
</commit_message>
<xml_diff>
--- a/3-2-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
+++ b/3-2-heritage-happenings/2025/04-april-hh/resident-directory/2025-04-heritage-resident-directory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348E1419F457EB2/Documents/GitHub/theo-armour-agenda/3-1-heritage/0-heritage-happenings/2025/04-april-hh/resident-directory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348E1419F457EB2/Documents/GitHub/theo-armour-agenda/3-2-heritage-happenings/2025/04-april-hh/resident-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1060" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A53FD7C9-5428-443F-BFB8-E910C86E3ABD}"/>
+  <xr:revisionPtr revIDLastSave="1069" documentId="8_{47523533-A004-48EF-BEEC-0FA3DE3C4717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8A9C1D9-3B4A-4901-BB8A-E0430A58C51A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="754" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Residents" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1197">
   <si>
     <t>First Name</t>
   </si>
@@ -3649,6 +3649,18 @@
   </si>
   <si>
     <t>Nancy O</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Sawyer</t>
+  </si>
+  <si>
+    <t>415 813-9973</t>
+  </si>
+  <si>
+    <t>georgesawyer@att.net</t>
   </si>
 </sst>
 </file>
@@ -4036,7 +4048,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9D9D9"/>
+          <bgColor rgb="FFD9D9D9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -4510,9 +4533,9 @@
   </sheetPr>
   <dimension ref="A1:J1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.15234375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6045,30 +6068,24 @@
         <v>312</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
-        <v>313</v>
+        <v>1193</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>71</v>
+        <v>1194</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>315</v>
+        <v>566</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="H61" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I61" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>317</v>
+        <v>1195</v>
+      </c>
+      <c r="F61" s="39" t="s">
+        <v>1196</v>
+      </c>
+      <c r="J61" s="16" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="13.5" x14ac:dyDescent="0.3">
@@ -9214,8 +9231,8 @@
       <c r="J1005" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:AB2 C3:I7 J3:AB18 C8:D9 F8:I9 C10:I11 C12:E12 H12:I12 C13:I18 C19:AB52 D53:E54 C55:AB76">
-    <cfRule type="expression" dxfId="22" priority="1">
+  <conditionalFormatting sqref="C2:AB2 C3:I7 J3:AB18 C8:D9 F8:I9 C10:I11 C12:E12 H12:I12 C13:I18 C19:AB52 D53:E54 C55:AB60 C62:AB76 D61:E61">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9242,9 +9259,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:K39"/>
+  <dimension ref="A2:K40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
@@ -9943,224 +9960,257 @@
     </row>
     <row r="30" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>71</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="F30" s="39"/>
-      <c r="G30" s="1" t="s">
+      <c r="F31" s="39"/>
+      <c r="G31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I31" s="4" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="32" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>595</v>
       </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>596</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>597</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="4" t="s">
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>599</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>601</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="10"/>
-      <c r="I32" s="1" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>610</v>
-      </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
         <v>605</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" s="1" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>612</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>613</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J36" s="5" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="13.5" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:11" ht="13.5" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:11" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>615</v>
       </c>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" s="17" customFormat="1" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
-      <c r="F38"/>
-      <c r="G38"/>
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38" s="16"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D40" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>618</v>
       </c>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
+      <c r="F40" s="1"/>
+      <c r="G40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="4" t="s">
+      <c r="H40" s="1"/>
+      <c r="I40" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>620</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8:AB8">
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:AC10 A13:AC13 K38:AC38 A39:J39">
-    <cfRule type="expression" dxfId="8" priority="12">
+  <conditionalFormatting sqref="A10:AC10 A13:AC13 K39:AC39 A40:J40">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18:AC18">
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:AC23">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:E12 G12:AA12">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:I15 K15:AB15 A27:J27">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="5" priority="10">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:AA2">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:AA11">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>"ISEVEN(ROW()"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24:AA24">
     <cfRule type="expression" dxfId="2" priority="5">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24:AA24">
-    <cfRule type="expression" dxfId="1" priority="4">
+  <conditionalFormatting sqref="C31:AA31">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:AA30">
+  <conditionalFormatting sqref="C30:AB30">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
@@ -10174,7 +10224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26C4F1CA-A107-47E1-B61D-684F7BB5060E}">
   <dimension ref="A1:Z173"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="B62" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showZeros="0" showRuler="0" view="pageLayout" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
@@ -11216,19 +11266,19 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="str">
-        <v>Ernie Sabini</v>
+        <v>George Sawyer</v>
       </c>
       <c r="B61" s="11" t="str">
-        <v>119 P</v>
+        <v>305 P</v>
       </c>
       <c r="C61" s="11" t="str">
-        <v>415 409-6040</v>
-      </c>
-      <c r="D61" s="11">
-        <v>0</v>
+        <v>415 813-9973</v>
+      </c>
+      <c r="D61" s="11" t="str">
+        <v>georgesawyer@att.net</v>
       </c>
       <c r="E61" s="11" t="str">
-        <v>03/22</v>
+        <v>08/23</v>
       </c>
     </row>
     <row r="62" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.35">
@@ -12734,12 +12784,12 @@
   </sheetData>
   <phoneticPr fontId="24" type="noConversion"/>
   <conditionalFormatting sqref="A2:E74">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="22" priority="1">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>ISEVEN(ROW())</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14553,52 +14603,52 @@
     <sortCondition ref="E2:E100"/>
   </sortState>
   <conditionalFormatting sqref="D17:D18">
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="18" priority="3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="18" priority="8">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D33">
-    <cfRule type="expression" dxfId="16" priority="10">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="16" priority="4">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:D96">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98:D100">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>"ISEVEN(ROW()"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>